<commit_message>
bug fixes and doc update
</commit_message>
<xml_diff>
--- a/input/general/GDP_per_capita_change_rate_projection.xlsx
+++ b/input/general/GDP_per_capita_change_rate_projection.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09720295-360A-43C1-9589-48831B4E20FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B307E53-B821-4A2D-9A12-B121C5C2D6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29145" yWindow="645" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="245">
   <si>
     <t>Country</t>
   </si>
@@ -160,12 +160,6 @@
     <t>2021-2030</t>
   </si>
   <si>
-    <t>2031-2040</t>
-  </si>
-  <si>
-    <t>2041-2050</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -764,6 +758,15 @@
   </si>
   <si>
     <t>The World in 2050, The Long View: How will the global economic order change by 2050?</t>
+  </si>
+  <si>
+    <t>2020-2030</t>
+  </si>
+  <si>
+    <t>2030-2040</t>
+  </si>
+  <si>
+    <t>2040-2050</t>
   </si>
 </sst>
 </file>
@@ -892,7 +895,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -907,11 +910,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1191,18 +1195,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1210,24 +1214,25 @@
         <v>40</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>41</v>
+        <v>242</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>243</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>244</v>
       </c>
       <c r="F1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
-        <v>1.3</v>
+      <c r="B2" s="13">
+        <f>C2</f>
+        <v>1.0799590923206592</v>
       </c>
       <c r="C2" s="11">
         <v>1.0799590923206592</v>
@@ -1239,15 +1244,16 @@
         <v>1.5</v>
       </c>
       <c r="F2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
-        <v>3.3</v>
+      <c r="B3" s="13">
+        <f t="shared" ref="B3:B39" si="0">C3</f>
+        <v>3.1006994595336623</v>
       </c>
       <c r="C3" s="11">
         <v>3.1006994595336623</v>
@@ -1259,15 +1265,16 @@
         <v>2.7</v>
       </c>
       <c r="F3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12">
-        <v>2.2999999999999998</v>
+      <c r="B4" s="13">
+        <f t="shared" si="0"/>
+        <v>2.8036619211585068</v>
       </c>
       <c r="C4" s="11">
         <v>2.8036619211585068</v>
@@ -1279,15 +1286,16 @@
         <v>1.75</v>
       </c>
       <c r="F4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12">
-        <v>1.8</v>
+      <c r="B5" s="13">
+        <f t="shared" si="0"/>
+        <v>1.5788050885373606</v>
       </c>
       <c r="C5" s="11">
         <v>1.5788050885373606</v>
@@ -1299,15 +1307,16 @@
         <v>1.8</v>
       </c>
       <c r="F5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
-        <v>0.8</v>
+      <c r="B6" s="13">
+        <f t="shared" si="0"/>
+        <v>1.3026326586460302</v>
       </c>
       <c r="C6" s="11">
         <v>1.3026326586460302</v>
@@ -1319,15 +1328,16 @@
         <v>1.8</v>
       </c>
       <c r="F6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12">
-        <v>3</v>
+      <c r="B7" s="13">
+        <f t="shared" si="0"/>
+        <v>3.1575706489613609</v>
       </c>
       <c r="C7" s="11">
         <v>3.1575706489613609</v>
@@ -1339,15 +1349,16 @@
         <v>3.1</v>
       </c>
       <c r="F7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="12">
-        <v>4.5999999999999996</v>
+      <c r="B8" s="13">
+        <f t="shared" si="0"/>
+        <v>3.4112691933074979</v>
       </c>
       <c r="C8" s="11">
         <v>3.4112691933074979</v>
@@ -1359,15 +1370,16 @@
         <v>1.4</v>
       </c>
       <c r="F8" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12">
-        <v>2.2999999999999998</v>
+      <c r="B9" s="13">
+        <f t="shared" si="0"/>
+        <v>1.7512423313889913</v>
       </c>
       <c r="C9" s="11">
         <v>1.7512423313889913</v>
@@ -1379,15 +1391,16 @@
         <v>1.7</v>
       </c>
       <c r="F9" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="12">
-        <v>1.8</v>
+      <c r="B10" s="13">
+        <f t="shared" si="0"/>
+        <v>2.0706815009670088</v>
       </c>
       <c r="C10" s="11">
         <v>2.0706815009670088</v>
@@ -1399,15 +1412,16 @@
         <v>1.4</v>
       </c>
       <c r="F10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="12">
-        <v>1.1000000000000001</v>
+      <c r="B11" s="13">
+        <f t="shared" si="0"/>
+        <v>1.4239992638658716</v>
       </c>
       <c r="C11" s="11">
         <v>1.4239992638658716</v>
@@ -1419,15 +1433,16 @@
         <v>1.6</v>
       </c>
       <c r="F11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="12">
-        <v>2.8</v>
+      <c r="B12" s="13">
+        <f t="shared" si="0"/>
+        <v>2.9194488076590641</v>
       </c>
       <c r="C12" s="11">
         <v>2.9194488076590641</v>
@@ -1439,15 +1454,16 @@
         <v>1.9</v>
       </c>
       <c r="F12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12">
-        <v>0.2</v>
+      <c r="B13" s="13">
+        <f t="shared" si="0"/>
+        <v>0.80879929151302932</v>
       </c>
       <c r="C13" s="11">
         <v>0.80879929151302932</v>
@@ -1459,15 +1475,16 @@
         <v>1.5</v>
       </c>
       <c r="F13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="12">
-        <v>3</v>
+      <c r="B14" s="13">
+        <f t="shared" si="0"/>
+        <v>2.713879318062018</v>
       </c>
       <c r="C14" s="11">
         <v>2.713879318062018</v>
@@ -1479,15 +1496,16 @@
         <v>2.1</v>
       </c>
       <c r="F14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="12">
-        <v>2.2000000000000002</v>
+      <c r="B15" s="13">
+        <f t="shared" si="0"/>
+        <v>3.0175636959453911</v>
       </c>
       <c r="C15" s="11">
         <v>3.0175636959453911</v>
@@ -1499,15 +1517,16 @@
         <v>3.2</v>
       </c>
       <c r="F15" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="12">
-        <v>3.2</v>
+      <c r="B16" s="13">
+        <f t="shared" si="0"/>
+        <v>2.2485003202490361</v>
       </c>
       <c r="C16" s="11">
         <v>2.2485003202490361</v>
@@ -1519,15 +1538,16 @@
         <v>2.5</v>
       </c>
       <c r="F16" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12">
-        <v>2.7</v>
+      <c r="B17" s="13">
+        <f t="shared" si="0"/>
+        <v>2.2274853447708631</v>
       </c>
       <c r="C17" s="11">
         <v>2.2274853447708631</v>
@@ -1541,15 +1561,16 @@
         <v>2.2274853447708631</v>
       </c>
       <c r="F17" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="12">
-        <v>1.6</v>
+      <c r="B18" s="13">
+        <f t="shared" si="0"/>
+        <v>2.7508281765034726</v>
       </c>
       <c r="C18" s="11">
         <v>2.7508281765034726</v>
@@ -1561,15 +1582,16 @@
         <v>1.75</v>
       </c>
       <c r="F18" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12">
-        <v>2.4</v>
+      <c r="B19" s="13">
+        <f t="shared" si="0"/>
+        <v>3.5033376749624701</v>
       </c>
       <c r="C19" s="11">
         <v>3.5033376749624701</v>
@@ -1581,15 +1603,16 @@
         <v>2.5</v>
       </c>
       <c r="F19" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="12">
-        <v>1.5</v>
+      <c r="B20" s="13">
+        <f t="shared" si="0"/>
+        <v>1.4410734195107855</v>
       </c>
       <c r="C20" s="11">
         <v>1.4410734195107855</v>
@@ -1601,15 +1624,16 @@
         <v>1.9</v>
       </c>
       <c r="F20" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="12">
-        <v>1.4</v>
+      <c r="B21" s="13">
+        <f t="shared" si="0"/>
+        <v>1.6194987396009441</v>
       </c>
       <c r="C21" s="11">
         <v>1.6194987396009441</v>
@@ -1621,15 +1645,16 @@
         <v>1.2</v>
       </c>
       <c r="F21" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="12">
-        <v>3.6</v>
+      <c r="B22" s="13">
+        <f t="shared" si="0"/>
+        <v>2.6806256436602949</v>
       </c>
       <c r="C22" s="11">
         <v>2.6806256436602949</v>
@@ -1641,15 +1666,16 @@
         <v>1.8</v>
       </c>
       <c r="F22" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="12">
-        <v>1.8</v>
+      <c r="B23" s="13">
+        <f t="shared" si="0"/>
+        <v>1.7981990890303834</v>
       </c>
       <c r="C23" s="11">
         <v>1.7981990890303834</v>
@@ -1661,15 +1687,16 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="F23" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="12">
-        <v>3.8</v>
+      <c r="B24" s="13">
+        <f t="shared" si="0"/>
+        <v>3.4719565162630639</v>
       </c>
       <c r="C24" s="11">
         <v>3.4719565162630639</v>
@@ -1681,15 +1708,16 @@
         <v>2.5</v>
       </c>
       <c r="F24" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="12">
-        <v>2.6</v>
+      <c r="B25" s="13">
+        <f t="shared" si="0"/>
+        <v>2.7202518057623859</v>
       </c>
       <c r="C25" s="11">
         <v>2.7202518057623859</v>
@@ -1701,15 +1729,16 @@
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="12">
-        <v>2.2000000000000002</v>
+      <c r="B26" s="13">
+        <f t="shared" si="0"/>
+        <v>2.77780149834288</v>
       </c>
       <c r="C26" s="11">
         <v>2.77780149834288</v>
@@ -1721,15 +1750,16 @@
         <v>2.5</v>
       </c>
       <c r="F26" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="12">
-        <v>1.5</v>
+      <c r="B27" s="13">
+        <f t="shared" si="0"/>
+        <v>1.1230224397165589</v>
       </c>
       <c r="C27" s="11">
         <v>1.1230224397165589</v>
@@ -1741,15 +1771,16 @@
         <v>1.4</v>
       </c>
       <c r="F27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="12">
-        <v>1.2</v>
+      <c r="B28" s="13">
+        <f t="shared" si="0"/>
+        <v>1.6417700656033984</v>
       </c>
       <c r="C28" s="11">
         <v>1.6417700656033984</v>
@@ -1761,15 +1792,16 @@
         <v>1.25</v>
       </c>
       <c r="F28" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="12">
-        <v>1.2</v>
+      <c r="B29" s="13">
+        <f t="shared" si="0"/>
+        <v>2.5434456719999998</v>
       </c>
       <c r="C29" s="11">
         <v>2.5434456719999998</v>
@@ -1781,15 +1813,16 @@
         <v>1.6</v>
       </c>
       <c r="F29" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="12">
-        <v>2.8</v>
+      <c r="B30" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4582591670348597</v>
       </c>
       <c r="C30" s="11">
         <v>2.4582591670348597</v>
@@ -1803,205 +1836,214 @@
         <v>2.4582591670348597</v>
       </c>
       <c r="F30" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="12">
-        <v>2.2000000000000002</v>
+      <c r="B31" s="13">
+        <f t="shared" si="0"/>
+        <v>1.7928633901420188</v>
       </c>
       <c r="C31" s="11">
         <v>1.7928633901420188</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" ref="D31:E39" si="0">C31</f>
+        <f t="shared" ref="D31:E39" si="1">C31</f>
         <v>1.7928633901420188</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7928633901420188</v>
       </c>
       <c r="F31" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="12">
-        <v>1.2</v>
+      <c r="B32" s="13">
+        <f t="shared" si="0"/>
+        <v>1.3592579970878038</v>
       </c>
       <c r="C32" s="11">
         <v>1.3592579970878038</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3592579970878038</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3592579970878038</v>
       </c>
       <c r="F32" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="12">
-        <v>2.5</v>
+      <c r="B33" s="13">
+        <f t="shared" si="0"/>
+        <v>2.8998052577562605</v>
       </c>
       <c r="C33" s="11">
         <v>2.8998052577562605</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8998052577562605</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8998052577562605</v>
       </c>
       <c r="F33" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="12">
-        <v>3.7</v>
+      <c r="B34" s="13">
+        <f t="shared" si="0"/>
+        <v>3.6554848536070939</v>
       </c>
       <c r="C34" s="11">
         <v>3.6554848536070939</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.6554848536070939</v>
       </c>
       <c r="E34" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.6554848536070939</v>
       </c>
       <c r="F34" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="12">
-        <v>4.0999999999999996</v>
+      <c r="B35" s="13">
+        <f t="shared" si="0"/>
+        <v>3.1394633785801984</v>
       </c>
       <c r="C35" s="11">
         <v>3.1394633785801984</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1394633785801984</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1394633785801984</v>
       </c>
       <c r="F35" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="12">
-        <v>3.7</v>
+      <c r="B36" s="13">
+        <f t="shared" si="0"/>
+        <v>3.747385816724802</v>
       </c>
       <c r="C36" s="11">
         <v>3.747385816724802</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.747385816724802</v>
       </c>
       <c r="E36" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.747385816724802</v>
       </c>
       <c r="F36" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="12">
-        <v>3.8</v>
+      <c r="B37" s="13">
+        <f t="shared" si="0"/>
+        <v>2.799218745533083</v>
       </c>
       <c r="C37" s="11">
         <v>2.799218745533083</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.799218745533083</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.799218745533083</v>
       </c>
       <c r="F37" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="12">
-        <v>3.8</v>
+      <c r="B38" s="13">
+        <f t="shared" si="0"/>
+        <v>3.6798380193440394</v>
       </c>
       <c r="C38" s="11">
         <v>3.6798380193440394</v>
       </c>
       <c r="D38" s="4">
+        <f t="shared" si="1"/>
+        <v>3.6798380193440394</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" si="1"/>
+        <v>3.6798380193440394</v>
+      </c>
+      <c r="F38" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="13">
         <f t="shared" si="0"/>
-        <v>3.6798380193440394</v>
-      </c>
-      <c r="E38" s="4">
-        <f t="shared" si="0"/>
-        <v>3.6798380193440394</v>
-      </c>
-      <c r="F38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="12">
         <v>3</v>
       </c>
       <c r="C39" s="4">
         <v>3</v>
       </c>
       <c r="D39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2017,32 +2059,32 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="5"/>
+    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -2050,98 +2092,98 @@
         <v>3.1394633785801984</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="5">
         <v>1.9925565393761779</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5">
         <v>1.9395173771644014</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="5">
         <v>3.8709321354974069</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="5">
         <v>4.0838842467734171</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="5">
         <v>2.0087994600641146</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" s="5">
         <v>4.2838950261899988</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" s="5">
         <v>1.3335333409080219</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" s="5">
         <v>2.0266540275533318</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2149,76 +2191,76 @@
         <v>1.6194987396009441</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="5">
         <v>2.5053971270810882</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" s="5">
         <v>2.4043156079286421</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" s="5">
         <v>3.0147972598006056</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B16" s="5">
         <v>6.5795224754157555</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B17" s="5">
         <v>2.9422323235527514</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" s="5">
         <v>0.6563923058663379</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2226,54 +2268,54 @@
         <v>1.0799590923206592</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" s="5">
         <v>2.009199846279941</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="5">
         <v>6.0473599603026784</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" s="5">
         <v>5.395469554591581</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B23" s="5">
         <v>2.8196811037813241</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2281,43 +2323,43 @@
         <v>2.799218745533083</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" s="5">
         <v>3.9743985985870811</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" s="5">
         <v>1.7781110994721905</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" s="5">
         <v>3.1494585313900592</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -2325,186 +2367,186 @@
         <v>3.1006994595336623</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" s="5">
         <v>5.1550781495696141</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B30" s="5">
         <v>4.6797648357325361</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B31" s="5">
         <v>5.0890373121091681</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B32" s="5">
         <v>6.4691143744759483</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B33" s="5">
         <v>4.8170829633246592</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B34" s="5">
         <v>1.7937561972953819</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B35" s="5">
         <v>3.6071294261492914</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B36" s="5">
         <v>3.4849856907312127</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B37" s="5">
         <v>1.6455576620901358</v>
       </c>
       <c r="C37" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B38" s="5">
         <v>4.5603715678763868</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B39" s="5">
         <v>2.9758145234572542</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B40" s="5">
         <v>4.0566362118912513</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B41" s="5">
         <v>6.7766052245409991</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B42" s="5">
         <v>3.3915207486342913</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B43" s="5">
         <v>3.1478756326285051</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B44" s="5">
         <v>6.3097628908674208</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2512,10 +2554,10 @@
         <v>2.9194488076590641</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2523,21 +2565,21 @@
         <v>2.713879318062018</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B47" s="5">
         <v>2.8036619211585068</v>
       </c>
       <c r="C47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -2545,98 +2587,98 @@
         <v>1.5788050885373606</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B49" s="5">
         <v>5.7948578290704544</v>
       </c>
       <c r="C49" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B50" s="5">
         <v>3.7170404030193893</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B51" s="5">
         <v>4.8982028071090866</v>
       </c>
       <c r="C51" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B52" s="5">
         <v>2.7697889209442161</v>
       </c>
       <c r="C52" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B53" s="5">
         <v>5.355012239332857</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B54" s="5">
         <v>1.8046801400966261</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B55" s="5">
         <v>-4.8396868564120288</v>
       </c>
       <c r="C55" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B56" s="5">
         <v>2.8875953765831852</v>
       </c>
       <c r="C56" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2644,43 +2686,43 @@
         <v>3.1575706489613609</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B58" s="5">
         <v>2.1697864038474401</v>
       </c>
       <c r="C58" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B59" s="5">
         <v>6.44782266381414</v>
       </c>
       <c r="C59" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B60" s="5">
         <v>5.1447173385441802</v>
       </c>
       <c r="C60" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -2688,10 +2730,10 @@
         <v>1.1230224397165589</v>
       </c>
       <c r="C61" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -2699,43 +2741,43 @@
         <v>1.4239992638658716</v>
       </c>
       <c r="C62" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B63" s="5">
         <v>3.7607954158812573</v>
       </c>
       <c r="C63" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B64" s="5">
         <v>5.6560539642912966</v>
       </c>
       <c r="C64" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B65" s="5">
         <v>4.958089999356563</v>
       </c>
       <c r="C65" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -2743,21 +2785,21 @@
         <v>1.3026326586460302</v>
       </c>
       <c r="C66" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B67" s="5">
         <v>4.8174167099427123</v>
       </c>
       <c r="C67" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -2765,98 +2807,98 @@
         <v>1.7512423313889913</v>
       </c>
       <c r="C68" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B69" s="5">
         <v>3.4115140433327085</v>
       </c>
       <c r="C69" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B70" s="5">
         <v>3.5437902237059005</v>
       </c>
       <c r="C70" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B71" s="5">
         <v>5.1982510539632099</v>
       </c>
       <c r="C71" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B72" s="5">
         <v>4.8998089777712028</v>
       </c>
       <c r="C72" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B73" s="5">
         <v>20.347432167461509</v>
       </c>
       <c r="C73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B74" s="5">
         <v>1.299207131108937</v>
       </c>
       <c r="C74" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B75" s="5">
         <v>3.7598766338030609</v>
       </c>
       <c r="C75" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B76" s="5">
         <v>3.0911074024187579</v>
       </c>
       <c r="C76" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>17</v>
       </c>
@@ -2864,10 +2906,10 @@
         <v>2.7508281765034726</v>
       </c>
       <c r="C77" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>29</v>
       </c>
@@ -2875,54 +2917,54 @@
         <v>2.4582591670348597</v>
       </c>
       <c r="C78" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B79" s="5">
         <v>6.4689590064784142</v>
       </c>
       <c r="C79" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B80" s="5">
         <v>5.2026926673858664</v>
       </c>
       <c r="C80" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B81" s="5">
         <v>2.0467999972561657</v>
       </c>
       <c r="C81" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B82" s="5">
         <v>2.6914955530726203</v>
       </c>
       <c r="C82" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -2930,21 +2972,21 @@
         <v>3.4112691933074979</v>
       </c>
       <c r="C83" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B84" s="5">
         <v>3.1638195123315782</v>
       </c>
       <c r="C84" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -2952,87 +2994,87 @@
         <v>0.80879929151302932</v>
       </c>
       <c r="C85" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B86" s="5">
         <v>2.0824541545120256</v>
       </c>
       <c r="C86" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B87" s="5">
         <v>0.95290057142918272</v>
       </c>
       <c r="C87" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B88" s="5">
         <v>3.1197203469055745</v>
       </c>
       <c r="C88" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B89" s="5">
         <v>3.5478565697210085</v>
       </c>
       <c r="C89" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B90" s="5">
         <v>5.4252327789016563</v>
       </c>
       <c r="C90" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B91" s="5">
         <v>2.32167462695263</v>
       </c>
       <c r="C91" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B92" s="5">
         <v>2.4383336994346028</v>
       </c>
       <c r="C92" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>37</v>
       </c>
@@ -3040,43 +3082,43 @@
         <v>3.6798380193440394</v>
       </c>
       <c r="C93" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B94" s="5">
         <v>2.6327960814251927</v>
       </c>
       <c r="C94" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B95" s="5">
         <v>3.7295887337195577</v>
       </c>
       <c r="C95" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B96" s="5">
         <v>3.8489602828523539</v>
       </c>
       <c r="C96" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -3084,51 +3126,51 @@
         <v>3.0175636959453911</v>
       </c>
       <c r="C97" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C98" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B99" s="5">
         <v>1.3804392594034098</v>
       </c>
       <c r="C99" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B100" s="5">
         <v>5.3213545713318711</v>
       </c>
       <c r="C100" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B101" s="5">
         <v>8.1761024270640803</v>
       </c>
       <c r="C101" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>15</v>
       </c>
@@ -3136,10 +3178,10 @@
         <v>2.2485003202490361</v>
       </c>
       <c r="C102" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -3147,76 +3189,76 @@
         <v>2.2274853447708631</v>
       </c>
       <c r="C103" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B104" s="5">
         <v>19.980682218942249</v>
       </c>
       <c r="C104" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B105" s="5">
         <v>5.084970188304716</v>
       </c>
       <c r="C105" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B106" s="5">
         <v>3.6928188430073838</v>
       </c>
       <c r="C106" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B107" s="5">
         <v>4.4179402153438074</v>
       </c>
       <c r="C107" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B108" s="5">
         <v>5.8590739691689153</v>
       </c>
       <c r="C108" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B109" s="5">
         <v>5.1119097685454307</v>
       </c>
       <c r="C109" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>18</v>
       </c>
@@ -3224,87 +3266,87 @@
         <v>3.5033376749624701</v>
       </c>
       <c r="C110" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B111" s="5">
         <v>2.0077521825225819</v>
       </c>
       <c r="C111" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B112" s="5">
         <v>5.8780438478969632</v>
       </c>
       <c r="C112" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B113" s="5">
         <v>3.9039275832589926</v>
       </c>
       <c r="C113" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B114" s="5">
         <v>1.8531090472304168</v>
       </c>
       <c r="C114" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B115" s="5">
         <v>1.6689205553142683</v>
       </c>
       <c r="C115" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B116" s="5">
         <v>4.6884732911316451</v>
       </c>
       <c r="C116" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B117" s="5">
         <v>5.6973600153161552</v>
       </c>
       <c r="C117" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>32</v>
       </c>
@@ -3312,76 +3354,76 @@
         <v>2.8998052577562605</v>
       </c>
       <c r="C118" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B119" s="5">
         <v>3.1383016306986367</v>
       </c>
       <c r="C119" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B120" s="5">
         <v>9.012874629561729</v>
       </c>
       <c r="C120" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B121" s="5">
         <v>3.3575212043992719</v>
       </c>
       <c r="C121" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B122" s="5">
         <v>2.67443200250288</v>
       </c>
       <c r="C122" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B123" s="5">
         <v>2.0099720515069919</v>
       </c>
       <c r="C123" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B124" s="5">
         <v>5.1759592248237896</v>
       </c>
       <c r="C124" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>19</v>
       </c>
@@ -3389,54 +3431,54 @@
         <v>1.4410734195107855</v>
       </c>
       <c r="C125" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B126" s="5">
         <v>2.1514572315447733</v>
       </c>
       <c r="C126" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B127" s="5">
         <v>3.5595626301230476</v>
       </c>
       <c r="C127" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B128" s="5">
         <v>7.975145647281856</v>
       </c>
       <c r="C128" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B129" s="5">
         <v>2.9293933936220817</v>
       </c>
       <c r="C129" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>33</v>
       </c>
@@ -3444,10 +3486,10 @@
         <v>3.6554848536070939</v>
       </c>
       <c r="C130" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>30</v>
       </c>
@@ -3455,98 +3497,98 @@
         <v>1.7928633901420188</v>
       </c>
       <c r="C131" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B132" s="5">
         <v>2.6913528441363521</v>
       </c>
       <c r="C132" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B133" s="5">
         <v>4.4584723657715486</v>
       </c>
       <c r="C133" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B134" s="5">
         <v>6.501137691589709</v>
       </c>
       <c r="C134" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B135" s="5">
         <v>4.4008202893085491</v>
       </c>
       <c r="C135" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B136" s="5">
         <v>3.3979293994828685</v>
       </c>
       <c r="C136" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B137" s="5">
         <v>3.6595075958649748</v>
       </c>
       <c r="C137" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B138" s="5">
         <v>2.9793936704469726</v>
       </c>
       <c r="C138" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B139" s="5">
         <v>5.7918889062514411</v>
       </c>
       <c r="C139" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>21</v>
       </c>
@@ -3554,10 +3596,10 @@
         <v>2.6806256436602949</v>
       </c>
       <c r="C140" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>22</v>
       </c>
@@ -3565,32 +3607,32 @@
         <v>1.7981990890303834</v>
       </c>
       <c r="C141" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B142" s="5">
         <v>-0.54252774039496021</v>
       </c>
       <c r="C142" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B143" s="5">
         <v>2.6894173430166424</v>
       </c>
       <c r="C143" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>23</v>
       </c>
@@ -3598,87 +3640,87 @@
         <v>3.4719565162630639</v>
       </c>
       <c r="C144" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B145" s="5">
         <v>0.33493540198030747</v>
       </c>
       <c r="C145" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B146" s="5">
         <v>6.663632192896185</v>
       </c>
       <c r="C146" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B147" s="5">
         <v>3.4845751280919712</v>
       </c>
       <c r="C147" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B148" s="5">
         <v>1.146772585322231</v>
       </c>
       <c r="C148" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B149" s="5">
         <v>3.5157162012907861</v>
       </c>
       <c r="C149" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B150" s="5">
         <v>3.0931906626552097</v>
       </c>
       <c r="C150" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B151" s="5">
         <v>6.6970919403634754</v>
       </c>
       <c r="C151" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>35</v>
       </c>
@@ -3686,54 +3728,54 @@
         <v>3.747385816724802</v>
       </c>
       <c r="C152" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B153" s="5">
         <v>4.4227723841651301</v>
       </c>
       <c r="C153" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B154" s="5">
         <v>4.3947084707022688</v>
       </c>
       <c r="C154" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B155" s="5">
         <v>2.4737307180819013</v>
       </c>
       <c r="C155" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B156" s="5">
         <v>2.77780149834288</v>
       </c>
       <c r="C156" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>24</v>
       </c>
@@ -3741,54 +3783,54 @@
         <v>2.7202518057623859</v>
       </c>
       <c r="C157" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B158" s="5">
         <v>2.773494869461568</v>
       </c>
       <c r="C158" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B159" s="5">
         <v>3.7555648736334435</v>
       </c>
       <c r="C159" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B160" s="5">
         <v>1.3099288835737743</v>
       </c>
       <c r="C160" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B161" s="5">
         <v>4.737854599996405</v>
       </c>
       <c r="C161" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>9</v>
       </c>
@@ -3796,76 +3838,76 @@
         <v>2.0706815009670088</v>
       </c>
       <c r="C162" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B163" s="5">
         <v>1.4153157632571745</v>
       </c>
       <c r="C163" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B164" s="5">
         <v>3.4428378319875108</v>
       </c>
       <c r="C164" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B165" s="5">
         <v>2.9376426382698106</v>
       </c>
       <c r="C165" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B166" s="5">
         <v>3.9320938899022106</v>
       </c>
       <c r="C166" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B167" s="5">
         <v>5.4776879955427127</v>
       </c>
       <c r="C167" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B168" s="5">
         <v>2.85848118716725</v>
       </c>
       <c r="C168" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>27</v>
       </c>
@@ -3873,10 +3915,10 @@
         <v>1.6417700656033984</v>
       </c>
       <c r="C169" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>31</v>
       </c>
@@ -3884,180 +3926,180 @@
         <v>1.3592579970878038</v>
       </c>
       <c r="C170" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C171" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B172" s="5">
         <v>2.9701043189999998</v>
       </c>
       <c r="C172" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B173" s="5">
         <v>4.9361100179999999</v>
       </c>
       <c r="C173" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B174" s="5">
         <v>5.8520867169999997</v>
       </c>
       <c r="C174" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B175" s="5">
         <v>3.0241067469999998</v>
       </c>
       <c r="C175" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B176" s="5">
         <v>2.7727865949999999</v>
       </c>
       <c r="C176" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B177" s="5">
         <v>6.1213260920000003</v>
       </c>
       <c r="C177" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B178" s="5">
         <v>1.0021556899999999</v>
       </c>
       <c r="C178" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B179" s="5">
         <v>2.2236730740000001</v>
       </c>
       <c r="C179" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B180" s="5">
         <v>2.4179824810000001</v>
       </c>
       <c r="C180" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B181" s="5">
         <v>4.4396851740000001</v>
       </c>
       <c r="C181" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B182" s="5">
         <v>2.2648067169999999</v>
       </c>
       <c r="C182" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B183" s="5">
         <v>3.432223247</v>
       </c>
       <c r="C183" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B184" s="5">
         <v>6.2969833409999998</v>
       </c>
       <c r="C184" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C185" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B186" s="5">
         <v>4.1526665989999998</v>
       </c>
       <c r="C186" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>28</v>
       </c>
@@ -4065,114 +4107,114 @@
         <v>2.5434456719999998</v>
       </c>
       <c r="C187" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B188" s="5">
         <v>2.1584616429999999</v>
       </c>
       <c r="C188" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B189" s="5">
         <v>3.254671476</v>
       </c>
       <c r="C189" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B190" s="5">
         <v>5.3269069250000003</v>
       </c>
       <c r="C190" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B191" s="5">
         <v>2.6572387100000001</v>
       </c>
       <c r="C191" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C192" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B193" s="5">
         <v>6.0690497729999997</v>
       </c>
       <c r="C193" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B194" s="5">
         <v>3.2848644349999998</v>
       </c>
       <c r="C194" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B195" s="5">
         <v>4.1432243399999997</v>
       </c>
       <c r="C195" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B196" s="5">
         <v>4.297845186</v>
       </c>
       <c r="C196" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B197" s="5">
         <v>3.527061335</v>
       </c>
       <c r="C197" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -4184,40 +4226,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="3" max="3" width="60.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" t="s">
         <v>229</v>
       </c>
-      <c r="B3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>40</v>
@@ -4225,109 +4267,109 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E6" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D6" t="s">
-        <v>237</v>
-      </c>
-      <c r="E6" t="s">
-        <v>223</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" s="10"/>
       <c r="D7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E8" t="s">
         <v>238</v>
-      </c>
-      <c r="E7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>220</v>
-      </c>
-      <c r="D8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E8" t="s">
-        <v>240</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="D9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E9" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" t="s">
         <v>222</v>
-      </c>
-      <c r="E10" t="s">
-        <v>224</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>